<commit_message>
add term request tracker issue links
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@85110 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/ClinEpi_metadata.xlsx
+++ b/Load/ontology/harmonization/ClinEpi_metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="3140" windowWidth="29840" windowHeight="15660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="discussion" sheetId="7" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="term request" sheetId="4" r:id="rId5"/>
     <sheet name="omrse" sheetId="5" r:id="rId6"/>
     <sheet name="values" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6245" uniqueCount="2311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6255" uniqueCount="2319">
   <si>
     <t>ID</t>
   </si>
@@ -6958,6 +6959,30 @@
   </si>
   <si>
     <t>shall we change it to laboratory findings? Or change laboratory finds to laboratory test? Question need to be discussed between Chris and Jie</t>
+  </si>
+  <si>
+    <t>Previous request</t>
+  </si>
+  <si>
+    <t>https://github.com/EnvironmentOntology/envo/issues/225</t>
+  </si>
+  <si>
+    <t>https://github.com/EnvironmentOntology/envo/issues/226</t>
+  </si>
+  <si>
+    <t>https://github.com/EnvironmentOntology/envo/issues/227</t>
+  </si>
+  <si>
+    <t>https://github.com/EnvironmentOntology/envo/issues/228</t>
+  </si>
+  <si>
+    <t>https://github.com/EnvironmentOntology/envo/issues/229</t>
+  </si>
+  <si>
+    <t>https://github.com/EnvironmentOntology/envo/issues/230</t>
+  </si>
+  <si>
+    <t>DOID</t>
   </si>
 </sst>
 </file>
@@ -7091,7 +7116,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="501">
+  <cellStyleXfs count="503">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7593,6 +7618,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -7622,7 +7649,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="501">
+  <cellStyles count="503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -7895,6 +7922,7 @@
     <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -8123,6 +8151,7 @@
     <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8454,7 +8483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -26703,13 +26732,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B117" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B122" sqref="B122"/>
+      <selection pane="bottomRight" activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -28051,6 +28080,54 @@
       </c>
       <c r="B122" t="s">
         <v>2033</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B131" t="s">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="B132" t="s">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="B133" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="B134" t="s">
+        <v>2315</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="B135" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="B136" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="B137" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>2318</v>
       </c>
     </row>
   </sheetData>
@@ -30582,4 +30659,23 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>